<commit_message>
prepared datasets on ebike
</commit_message>
<xml_diff>
--- a/data-raw/contents.xlsx
+++ b/data-raw/contents.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t xml:space="preserve">Chapter</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">1F-nL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The e-bike frame hardening process</t>
   </si>
   <si>
     <t xml:space="preserve">plasma</t>
@@ -421,7 +424,7 @@
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -647,127 +650,130 @@
       <c r="B12" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="E12" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F23" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added solar panel dataset
</commit_message>
<xml_diff>
--- a/data-raw/contents.xlsx
+++ b/data-raw/contents.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="74">
   <si>
     <t xml:space="preserve">Chapter</t>
   </si>
   <si>
-    <t xml:space="preserve">Session</t>
+    <t xml:space="preserve">Unit</t>
   </si>
   <si>
     <t xml:space="preserve">Case</t>
@@ -40,13 +40,13 @@
     <t xml:space="preserve">Functions</t>
   </si>
   <si>
-    <t xml:space="preserve">Case Study Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case Study Storyline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dataset in Package</t>
+    <t xml:space="preserve">Photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storyline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data_packaged</t>
   </si>
   <si>
     <t xml:space="preserve">Six Sigma</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Precision</t>
   </si>
   <si>
-    <t xml:space="preserve">The pharmaceutical tablet compaction process</t>
+    <t xml:space="preserve">The tablet compaction process</t>
   </si>
   <si>
     <t xml:space="preserve">Pharma</t>
@@ -157,67 +157,73 @@
     <t xml:space="preserve">The e-bike frame hardening process</t>
   </si>
   <si>
+    <t xml:space="preserve">Bicycle manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ebike_hardening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats::lm](#linearModel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[car::durbinWatsonTest](#residualsCorrelation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats::bartlett.test](#barlettTest)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats::shapiro.test](#shapiroTest)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats::TukeyHSD](#tukeyTest)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[agricolae::LSD.test](#fisherLSD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats::predict](#predict)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2F-nL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[car::outlierTest](#outlierTest)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats::cor.test](#corTest)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2F-nL ancova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filament</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3F-nL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soft drink bottling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats::aov](#anova)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats:interaction.plot](#interactionPlot)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2F-2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chemical experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3F-2L</t>
+  </si>
+  <si>
     <t xml:space="preserve">plasma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats::lm](#linearModel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[car::durbinWatsonTest](#residualsCorrelation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats::bartlett.test](#barlettTest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats::shapiro.test](#shapiroTest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats::TukeyHSD](#tukeyTest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[agricolae::LSD.test](#fisherLSD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats::predict](#predict)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2F-nL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">battery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[car::outlierTest](#outlierTest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats::cor.test](#corTest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2F-nL ancova</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filament</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3F-nL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soft drink bottling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats::aov](#anova)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats:interaction.plot](#interactionPlot)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2F-2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chemical experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3F-2L</t>
   </si>
   <si>
     <t xml:space="preserve">mF-2L single replicate</t>
@@ -250,6 +256,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -271,6 +278,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -424,20 +432,20 @@
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.26"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -500,16 +508,49 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
       <c r="F3" s="0" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="0" t="s">
         <v>19</v>
       </c>
@@ -530,6 +571,9 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="B6" s="0" t="s">
         <v>22</v>
       </c>
@@ -553,8 +597,20 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="B7" s="0" t="s">
         <v>26</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>27</v>
@@ -593,6 +649,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B9" s="0" t="s">
         <v>33</v>
       </c>
@@ -613,9 +672,21 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B10" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="G10" s="0" t="s">
         <v>27</v>
       </c>
@@ -647,133 +718,265 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B12" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="D12" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="E12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="F14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="F15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="F16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="F17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="F18" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B19" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="E20" s="0" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B21" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B22" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E22" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="E23" s="0" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F23" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B24" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B25" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B26" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted non needed data files
</commit_message>
<xml_diff>
--- a/data-raw/contents.xlsx
+++ b/data-raw/contents.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="77">
   <si>
     <t xml:space="preserve">Chapter</t>
   </si>
@@ -187,10 +187,19 @@
     <t xml:space="preserve">2F-nL</t>
   </si>
   <si>
+    <t xml:space="preserve">The solar cell ouput test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solarcell_output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[car::outlierTest](#outlierTest)</t>
+  </si>
+  <si>
     <t xml:space="preserve">battery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[car::outlierTest](#outlierTest)</t>
   </si>
   <si>
     <t xml:space="preserve">[stats::cor.test](#corTest)</t>
@@ -432,7 +441,7 @@
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -864,11 +873,17 @@
       <c r="B19" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="C19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>56</v>
+      </c>
       <c r="E19" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,10 +894,10 @@
         <v>54</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,10 +905,10 @@
         <v>38</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,13 +916,13 @@
         <v>38</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,13 +930,13 @@
         <v>38</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,10 +944,10 @@
         <v>38</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,10 +955,10 @@
         <v>38</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,32 +966,32 @@
         <v>38</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated color in theme
</commit_message>
<xml_diff>
--- a/data-raw/contents.xlsx
+++ b/data-raw/contents.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="90">
   <si>
     <t xml:space="preserve">Chapter</t>
   </si>
@@ -64,93 +64,108 @@
     <t xml:space="preserve">dial_control</t>
   </si>
   <si>
+    <t xml:space="preserve">[qicharts2::paretochart](#paretochart)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ishikawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dental prosthesis Laboratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[qcc::cause.and.effect](#fishbone)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The perfume destilation experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perfume_experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ggplot2::geom_tile](#tileplot)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gage r&amp;R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linearity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The juice production plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juice_bottling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The tablet compaction process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tablet_thickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[SixSigma::ss.rr](#gageRnR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On going</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1F-2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The winter sports clothing manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pet_delivery</t>
+  </si>
+  <si>
     <t xml:space="preserve">[stats::t.test](#tTest)</t>
   </si>
   <si>
-    <t xml:space="preserve">ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completed</t>
-  </si>
-  <si>
     <t xml:space="preserve">[stats::var.test](#FTest)</t>
   </si>
   <si>
     <t xml:space="preserve">[car::leveneTest](#leveneTest)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ishikawa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The dental prosthesis Laboratory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Correlation Matrix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The perfume destilation experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perfume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">perfume_experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network clustering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gage r&amp;R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linearity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The juice production plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juice_bottling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The tablet compaction process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pharma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tablet_thickness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1F-2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The winter sports clothing manufacturer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clothing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pet_delivery</t>
-  </si>
-  <si>
     <t xml:space="preserve">1F-nL</t>
   </si>
   <si>
@@ -166,6 +181,9 @@
     <t xml:space="preserve">[stats::lm](#linearModel)</t>
   </si>
   <si>
+    <t xml:space="preserve">[broom::augment](#augment)</t>
+  </si>
+  <si>
     <t xml:space="preserve">[car::durbinWatsonTest](#residualsCorrelation)</t>
   </si>
   <si>
@@ -175,6 +193,12 @@
     <t xml:space="preserve">[stats::shapiro.test](#shapiroTest)</t>
   </si>
   <si>
+    <t xml:space="preserve">[car::outlierTest](#outlierTest)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[stats::aov](#anova)</t>
+  </si>
+  <si>
     <t xml:space="preserve">[stats::TukeyHSD](#tukeyTest)</t>
   </si>
   <si>
@@ -196,33 +220,27 @@
     <t xml:space="preserve">solarcell_output</t>
   </si>
   <si>
-    <t xml:space="preserve">[car::outlierTest](#outlierTest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">battery</t>
+    <t xml:space="preserve">[stats:interaction.plot](#interactionPlot)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2F-nL ancova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filament</t>
   </si>
   <si>
     <t xml:space="preserve">[stats::cor.test](#corTest)</t>
   </si>
   <si>
-    <t xml:space="preserve">2F-nL ancova</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filament</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3F-nL</t>
+    <t xml:space="preserve">[stats::aov – ancova](#ancova)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mF-nL</t>
   </si>
   <si>
     <t xml:space="preserve">soft drink bottling</t>
   </si>
   <si>
-    <t xml:space="preserve">[stats::aov](#anova)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[stats:interaction.plot](#interactionPlot)</t>
-  </si>
-  <si>
     <t xml:space="preserve">2F-2L</t>
   </si>
   <si>
@@ -235,12 +253,21 @@
     <t xml:space="preserve">plasma</t>
   </si>
   <si>
+    <t xml:space="preserve">[broom::glance](#glance)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[graphics::persp](#persp)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mF-2L single replicate</t>
   </si>
   <si>
     <t xml:space="preserve">filtration</t>
   </si>
   <si>
+    <t xml:space="preserve">[car::qqPlot](#qqPlot)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPC</t>
   </si>
   <si>
@@ -250,7 +277,19 @@
     <t xml:space="preserve">bamako</t>
   </si>
   <si>
+    <t xml:space="preserve">[qcc::qcc – xbar](#xbarchart)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[qcc::qcc – R](#Rchart)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[qcc::limits.xbar](#limitsxbar)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Capability Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[qcc::process.capability](#processcapability)</t>
   </si>
 </sst>
 </file>
@@ -260,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -285,6 +324,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -344,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -361,6 +407,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,7 +424,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -438,13 +488,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ28"/>
+  <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.65"/>
@@ -452,9 +502,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.27"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -521,19 +571,28 @@
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,19 +600,28 @@
         <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,16 +629,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>16</v>
@@ -581,19 +652,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>15</v>
@@ -607,25 +678,28 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>15</v>
@@ -636,22 +710,22 @@
         <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>15</v>
@@ -659,22 +733,28 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>15</v>
@@ -682,316 +762,618 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>60</v>
       </c>
+      <c r="G20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>62</v>
+      <c r="G21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>63</v>
       </c>
+      <c r="D22" s="0" t="s">
+        <v>64</v>
+      </c>
       <c r="E22" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="0" t="s">
         <v>75</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E28" s="0" t="s">
-        <v>75</v>
+      <c r="F28" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="4"/>
+      <c r="F32" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>